<commit_message>
Clean up tasks, evaluation
</commit_message>
<xml_diff>
--- a/data-viz/schedule.xlsx
+++ b/data-viz/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airwin/Dropbox/Teaching/STAT 2430 Data Viz/Data-Viz-2022/Course/data-viz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F705631-D779-2540-9513-3CD9C3B4DF29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C010EB28-27A0-5A40-8976-EC72C79880F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5720" yWindow="2300" windowWidth="28480" windowHeight="20880" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="30220" windowHeight="19220" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="187">
   <si>
     <t>Date</t>
   </si>
@@ -45,12 +45,6 @@
     <t>Lesson</t>
   </si>
   <si>
-    <t>Video</t>
-  </si>
-  <si>
-    <t>Title</t>
-  </si>
-  <si>
     <t>Invitation</t>
   </si>
   <si>
@@ -60,84 +54,39 @@
     <t>Computer tools</t>
   </si>
   <si>
-    <t>Notes</t>
-  </si>
-  <si>
     <t>Day</t>
   </si>
   <si>
-    <t>Agenda</t>
-  </si>
-  <si>
     <t>Accessing computer tools</t>
   </si>
   <si>
     <t>Look at data</t>
   </si>
   <si>
-    <t>notes_link</t>
-  </si>
-  <si>
     <t>slides_link</t>
   </si>
   <si>
-    <t>tasks_link</t>
-  </si>
-  <si>
     <t>Slides</t>
   </si>
   <si>
-    <t>Task 1</t>
-  </si>
-  <si>
-    <t>Bonus task</t>
-  </si>
-  <si>
-    <t>Task 2</t>
-  </si>
-  <si>
-    <t>Task 3</t>
-  </si>
-  <si>
     <t>slides</t>
   </si>
   <si>
-    <t>tasks</t>
-  </si>
-  <si>
-    <t>notes</t>
-  </si>
-  <si>
     <t>slides/00-course-mechanics.html</t>
   </si>
   <si>
-    <t>#welcome</t>
-  </si>
-  <si>
-    <t>#ch-invitation</t>
-  </si>
-  <si>
     <t>slides/01-invitation.html</t>
   </si>
   <si>
     <t>#task-1</t>
   </si>
   <si>
-    <t>#ch-tools</t>
-  </si>
-  <si>
     <t>slides/02-computer-tools.html</t>
   </si>
   <si>
     <t>#task-b1</t>
   </si>
   <si>
-    <t>#setup</t>
-  </si>
-  <si>
-    <t>#look-data</t>
-  </si>
-  <si>
     <t>slides/04-look-at-data.html</t>
   </si>
   <si>
@@ -150,9 +99,6 @@
     <t>Making your first plot</t>
   </si>
   <si>
-    <t>#first-plot</t>
-  </si>
-  <si>
     <t>slides/05-making-your-first-plot.html</t>
   </si>
   <si>
@@ -165,54 +111,27 @@
     <t>Version control</t>
   </si>
   <si>
-    <t>#vcs</t>
-  </si>
-  <si>
     <t>slides/06-version-control.html</t>
   </si>
   <si>
-    <t>#task-4</t>
-  </si>
-  <si>
     <t>Introduction to the grammar of graphics</t>
   </si>
   <si>
-    <t>#ggplot</t>
-  </si>
-  <si>
-    <t>#grammar</t>
-  </si>
-  <si>
     <t>Using the grammar of graphics</t>
   </si>
   <si>
     <t>#task-b2</t>
   </si>
   <si>
-    <t>Task 4</t>
-  </si>
-  <si>
-    <t>Task 5</t>
-  </si>
-  <si>
     <t>#task-5</t>
   </si>
   <si>
-    <t>Task 6</t>
-  </si>
-  <si>
     <t>#task-6</t>
   </si>
   <si>
-    <t>Task 7</t>
-  </si>
-  <si>
     <t>#task-7</t>
   </si>
   <si>
-    <t>Task 8</t>
-  </si>
-  <si>
     <t>#task-8</t>
   </si>
   <si>
@@ -279,12 +198,6 @@
     <t>slides/07-grammar-graphics.html</t>
   </si>
   <si>
-    <t>#summarizing-data</t>
-  </si>
-  <si>
-    <t>#reading-data</t>
-  </si>
-  <si>
     <t>Displaying tables</t>
   </si>
   <si>
@@ -294,27 +207,15 @@
     <t>slides/11-reading-data.html</t>
   </si>
   <si>
-    <t>#facets</t>
-  </si>
-  <si>
     <t>slides/09-facets.html</t>
   </si>
   <si>
     <t>#task-b5</t>
   </si>
   <si>
-    <t>#pivot</t>
-  </si>
-  <si>
-    <t>#format-tables</t>
-  </si>
-  <si>
     <t>Getting help</t>
   </si>
   <si>
-    <t>#help</t>
-  </si>
-  <si>
     <t>#task-b6</t>
   </si>
   <si>
@@ -327,12 +228,6 @@
     <t>slides/14-getting-help.html</t>
   </si>
   <si>
-    <t>#working-models</t>
-  </si>
-  <si>
-    <t>#linear-models</t>
-  </si>
-  <si>
     <t>Project teams sign-up deadline</t>
   </si>
   <si>
@@ -345,15 +240,6 @@
     <t>slides/17-gam-loess.html</t>
   </si>
   <si>
-    <t>#smoothing</t>
-  </si>
-  <si>
-    <t>Task 9</t>
-  </si>
-  <si>
-    <t>Task 10</t>
-  </si>
-  <si>
     <t>Collaboration with GitHub</t>
   </si>
   <si>
@@ -366,12 +252,6 @@
     <t>#task-10</t>
   </si>
   <si>
-    <t>#collaboration</t>
-  </si>
-  <si>
-    <t>Task 11</t>
-  </si>
-  <si>
     <t>#task-11</t>
   </si>
   <si>
@@ -387,12 +267,6 @@
     <t>#task-12</t>
   </si>
   <si>
-    <t>Task 12</t>
-  </si>
-  <si>
-    <t>#mds</t>
-  </si>
-  <si>
     <t>Finding data</t>
   </si>
   <si>
@@ -408,69 +282,30 @@
     <t>Alternatives to maps</t>
   </si>
   <si>
-    <t>#slides</t>
-  </si>
-  <si>
-    <t>#mapping-1</t>
-  </si>
-  <si>
-    <t>#k-means</t>
-  </si>
-  <si>
-    <t>#factors-dates</t>
-  </si>
-  <si>
-    <t>#colour</t>
-  </si>
-  <si>
     <t>Dynamic graphics</t>
   </si>
   <si>
     <t>Reconstructing a visualization</t>
   </si>
   <si>
-    <t>#theme</t>
-  </si>
-  <si>
     <t>slides/35-step-by-step.html</t>
   </si>
   <si>
-    <t>#output-files</t>
-  </si>
-  <si>
-    <t>Task 13</t>
-  </si>
-  <si>
     <t>#task-13</t>
   </si>
   <si>
     <t>#task-14</t>
   </si>
   <si>
-    <t>Task 14</t>
-  </si>
-  <si>
     <t>#task-b9</t>
   </si>
   <si>
-    <t>Task 15</t>
-  </si>
-  <si>
-    <t>Task 16</t>
-  </si>
-  <si>
     <t>#task-15</t>
   </si>
   <si>
     <t>#task-16</t>
   </si>
   <si>
-    <t>Task 17</t>
-  </si>
-  <si>
-    <t>Task 18</t>
-  </si>
-  <si>
     <t>#task-b10</t>
   </si>
   <si>
@@ -480,21 +315,6 @@
     <t>#task-18</t>
   </si>
   <si>
-    <t>#data-sources</t>
-  </si>
-  <si>
-    <t>#reproduce</t>
-  </si>
-  <si>
-    <t>#pca</t>
-  </si>
-  <si>
-    <t>#mapping-3</t>
-  </si>
-  <si>
-    <t>#mapping-2</t>
-  </si>
-  <si>
     <t>slides/20-MDS.html</t>
   </si>
   <si>
@@ -507,9 +327,6 @@
     <t>slides/25-testing.html</t>
   </si>
   <si>
-    <t>#testing</t>
-  </si>
-  <si>
     <t>Checking your work</t>
   </si>
   <si>
@@ -519,12 +336,6 @@
     <t>slides/18b-reproducible-reports.html</t>
   </si>
   <si>
-    <t>https://dal.hosted.panopto.com/Panopto/Pages/Viewer.aspx?id=09743375-5dbd-435e-ae66-ace000173c94</t>
-  </si>
-  <si>
-    <t>#dynamic</t>
-  </si>
-  <si>
     <t>slides/26-dynamic-graphics.html</t>
   </si>
   <si>
@@ -552,12 +363,6 @@
     <t>https://github.com/Dalhousie-AndrewIrwin-Teaching/team-planning/blob/main/presentation-schedule.csv</t>
   </si>
   <si>
-    <t>https://github.com/Dalhousie-AndrewIrwin-Teaching/team-planning/blob/main/peer-evaluation-schedule.csv</t>
-  </si>
-  <si>
-    <t>Peer evaluation</t>
-  </si>
-  <si>
     <t>Schedule</t>
   </si>
   <si>
@@ -577,6 +382,219 @@
   </si>
   <si>
     <t>Assignment 6 due</t>
+  </si>
+  <si>
+    <t>Setting up</t>
+  </si>
+  <si>
+    <t>Look</t>
+  </si>
+  <si>
+    <t>Summarize</t>
+  </si>
+  <si>
+    <t>Facets</t>
+  </si>
+  <si>
+    <t>Reshape</t>
+  </si>
+  <si>
+    <t>Tables</t>
+  </si>
+  <si>
+    <t>Collaboration</t>
+  </si>
+  <si>
+    <t>Reports</t>
+  </si>
+  <si>
+    <t>Maps</t>
+  </si>
+  <si>
+    <t>Map alternatives</t>
+  </si>
+  <si>
+    <t>lessons/101-introduction.html</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>title_link</t>
+  </si>
+  <si>
+    <t>lessons/102-intro-to-r.html</t>
+  </si>
+  <si>
+    <t>lessons/103-setup.html</t>
+  </si>
+  <si>
+    <t>lessons/104-look-at-data.html</t>
+  </si>
+  <si>
+    <t>lessons/105-first-plot.html</t>
+  </si>
+  <si>
+    <t>lessons/106-version-control.html</t>
+  </si>
+  <si>
+    <t>lessons/107-grammar-graphics.html</t>
+  </si>
+  <si>
+    <t>lessons/108-ggplot.html</t>
+  </si>
+  <si>
+    <t>lessons/110-summarizing-data.html</t>
+  </si>
+  <si>
+    <t>lessons/115-facets.html</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>lessons/111-reading-data.html</t>
+  </si>
+  <si>
+    <t>lessons/112-reshaping-data.html</t>
+  </si>
+  <si>
+    <t>lessons/113-data-tables.html</t>
+  </si>
+  <si>
+    <t>lessons/114-asking-questions.html</t>
+  </si>
+  <si>
+    <t>lessons/118-working-with-models.html</t>
+  </si>
+  <si>
+    <t>lessons/119-linear-models.html</t>
+  </si>
+  <si>
+    <t>lessons/120-gam-loess.html</t>
+  </si>
+  <si>
+    <t>lessons/124-collaboration.html</t>
+  </si>
+  <si>
+    <t>lessons/301-data-sources.html</t>
+  </si>
+  <si>
+    <t>lessons/133-reproducible-reports.html</t>
+  </si>
+  <si>
+    <t>lessons/121-PCA.html</t>
+  </si>
+  <si>
+    <t>lessons/122-mds.html</t>
+  </si>
+  <si>
+    <t>lessons/123-kmean.html</t>
+  </si>
+  <si>
+    <t>lessons/125-slides.html</t>
+  </si>
+  <si>
+    <t>lessons/127-test-data.html</t>
+  </si>
+  <si>
+    <t>lessons/155-dynamics-graphics.html</t>
+  </si>
+  <si>
+    <t>lessons/140-mapping.html</t>
+  </si>
+  <si>
+    <t>lessons/141-mapping-2.html</t>
+  </si>
+  <si>
+    <t>lessons/142-mapping-3.html</t>
+  </si>
+  <si>
+    <t>lessons/130-bonus-topics.html</t>
+  </si>
+  <si>
+    <t>lessons/201-colour.html</t>
+  </si>
+  <si>
+    <t>lessons/133-themes.html</t>
+  </si>
+  <si>
+    <t>lessons/130-graphics-output.html</t>
+  </si>
+  <si>
+    <t>lessons/134-reconstruction.html</t>
+  </si>
+  <si>
+    <t>LOESS-GAM</t>
+  </si>
+  <si>
+    <t>Team Planning</t>
+  </si>
+  <si>
+    <t>#task-planning</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;Bonus task&lt;/i&gt;</t>
+  </si>
+  <si>
+    <t>Proposal</t>
+  </si>
+  <si>
+    <t>Assignment 1</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>Assignment 2</t>
+  </si>
+  <si>
+    <t>Assignment 3</t>
+  </si>
+  <si>
+    <t>Assignment 4</t>
+  </si>
+  <si>
+    <t>Assignment 5</t>
+  </si>
+  <si>
+    <t>Assignment 6</t>
+  </si>
+  <si>
+    <t>#assignment-1</t>
+  </si>
+  <si>
+    <t>#assignment-2</t>
+  </si>
+  <si>
+    <t>#assignment-3</t>
+  </si>
+  <si>
+    <t>#assignment-4</t>
+  </si>
+  <si>
+    <t>#assignment-5</t>
+  </si>
+  <si>
+    <t>#assignment-6</t>
+  </si>
+  <si>
+    <t>#written-report</t>
+  </si>
+  <si>
+    <t>#proposal</t>
+  </si>
+  <si>
+    <t>evaluation</t>
+  </si>
+  <si>
+    <t>evaluation_link</t>
+  </si>
+  <si>
+    <t>#task-14a</t>
+  </si>
+  <si>
+    <t>Presentation</t>
   </si>
 </sst>
 </file>
@@ -586,10 +604,23 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="ddd\ dd\ mmm"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -615,9 +646,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -932,13 +964,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5054E2AF-B146-EF4C-9336-1C427A68EF7D}">
-  <dimension ref="A1:K47"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E6" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E13" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D48" sqref="D48"/>
+      <selection pane="bottomRight" activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -946,48 +978,44 @@
     <col min="1" max="1" width="6.83203125" customWidth="1"/>
     <col min="2" max="2" width="4.6640625" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.1640625" customWidth="1"/>
-    <col min="5" max="5" width="7" customWidth="1"/>
-    <col min="9" max="9" width="13.83203125" customWidth="1"/>
+    <col min="4" max="5" width="28.1640625" customWidth="1"/>
+    <col min="6" max="6" width="7" customWidth="1"/>
     <col min="10" max="10" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>4</v>
+        <v>127</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>128</v>
       </c>
       <c r="F1" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>183</v>
       </c>
       <c r="H1" t="s">
-        <v>22</v>
+        <v>184</v>
       </c>
       <c r="I1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -999,25 +1027,22 @@
         <v>44810</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F2">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
       <c r="I2" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="J2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1029,31 +1054,28 @@
         <v>44810</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F3">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
       <c r="G3" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="I3" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="J3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1065,31 +1087,28 @@
         <v>44812</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="F4" t="s">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="E4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
       </c>
       <c r="G4" t="s">
+        <v>166</v>
+      </c>
+      <c r="H4" t="s">
         <v>16</v>
       </c>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
       <c r="I4" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="J4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1101,25 +1120,22 @@
         <v>44812</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F5">
         <v>3</v>
       </c>
-      <c r="F5" t="s">
-        <v>8</v>
+      <c r="G5" t="s">
+        <v>116</v>
       </c>
       <c r="H5" t="s">
         <v>19</v>
       </c>
-      <c r="I5" t="s">
-        <v>32</v>
-      </c>
-      <c r="K5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1131,67 +1147,61 @@
         <v>44817</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>131</v>
+      </c>
+      <c r="F6">
         <v>4</v>
       </c>
-      <c r="F6" t="s">
-        <v>8</v>
-      </c>
       <c r="G6" t="s">
-        <v>16</v>
+        <v>117</v>
       </c>
       <c r="H6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1">
+        <f t="shared" si="0"/>
+        <v>44817</v>
+      </c>
+      <c r="D7" t="s">
         <v>20</v>
       </c>
-      <c r="I6" t="s">
-        <v>33</v>
-      </c>
-      <c r="J6" t="s">
-        <v>34</v>
-      </c>
-      <c r="K6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1">
-        <f t="shared" si="0"/>
-        <v>44817</v>
-      </c>
-      <c r="D7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7">
+      <c r="E7" t="s">
+        <v>132</v>
+      </c>
+      <c r="F7">
         <v>5</v>
       </c>
-      <c r="F7" t="s">
-        <v>8</v>
-      </c>
       <c r="G7" t="s">
-        <v>16</v>
+        <v>166</v>
       </c>
       <c r="H7" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="I7" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="J7" t="s">
-        <v>39</v>
-      </c>
-      <c r="K7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1203,31 +1213,22 @@
         <v>44819</v>
       </c>
       <c r="D8" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8">
+        <v>24</v>
+      </c>
+      <c r="E8" t="s">
+        <v>133</v>
+      </c>
+      <c r="F8">
         <v>6</v>
       </c>
-      <c r="F8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H8" t="s">
-        <v>51</v>
-      </c>
       <c r="I8" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="J8" t="s">
-        <v>44</v>
-      </c>
-      <c r="K8" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1239,31 +1240,28 @@
         <v>44824</v>
       </c>
       <c r="D9" t="s">
-        <v>46</v>
-      </c>
-      <c r="E9">
+        <v>26</v>
+      </c>
+      <c r="E9" t="s">
+        <v>134</v>
+      </c>
+      <c r="F9">
         <v>7</v>
       </c>
-      <c r="F9" t="s">
-        <v>8</v>
-      </c>
       <c r="G9" t="s">
-        <v>16</v>
+        <v>166</v>
       </c>
       <c r="H9" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="I9" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="J9" t="s">
-        <v>80</v>
-      </c>
-      <c r="K9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1275,31 +1273,28 @@
         <v>44824</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10">
+        <v>27</v>
+      </c>
+      <c r="E10" t="s">
+        <v>135</v>
+      </c>
+      <c r="F10">
         <v>8</v>
       </c>
-      <c r="F10" t="s">
-        <v>8</v>
-      </c>
       <c r="G10" t="s">
-        <v>16</v>
+        <v>166</v>
       </c>
       <c r="H10" t="s">
-        <v>18</v>
+        <v>51</v>
       </c>
       <c r="I10" t="s">
-        <v>47</v>
+        <v>10</v>
       </c>
       <c r="J10" t="s">
-        <v>79</v>
-      </c>
-      <c r="K10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>4</v>
       </c>
@@ -1311,31 +1306,28 @@
         <v>44831</v>
       </c>
       <c r="D11" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11">
+        <v>33</v>
+      </c>
+      <c r="E11" t="s">
+        <v>136</v>
+      </c>
+      <c r="F11">
         <v>9</v>
       </c>
-      <c r="F11" t="s">
-        <v>8</v>
-      </c>
       <c r="G11" t="s">
-        <v>16</v>
+        <v>118</v>
       </c>
       <c r="H11" t="s">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="I11" t="s">
-        <v>81</v>
+        <v>10</v>
       </c>
       <c r="J11" t="s">
-        <v>84</v>
-      </c>
-      <c r="K11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>4</v>
       </c>
@@ -1347,31 +1339,28 @@
         <v>44831</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12">
-        <v>10</v>
-      </c>
-      <c r="F12" t="s">
-        <v>8</v>
+        <v>36</v>
+      </c>
+      <c r="E12" t="s">
+        <v>137</v>
+      </c>
+      <c r="F12">
+        <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>16</v>
+        <v>119</v>
       </c>
       <c r="H12" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="I12" t="s">
-        <v>86</v>
+        <v>10</v>
       </c>
       <c r="J12" t="s">
-        <v>87</v>
-      </c>
-      <c r="K12" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1383,31 +1372,28 @@
         <v>44833</v>
       </c>
       <c r="D13" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13">
+        <v>34</v>
+      </c>
+      <c r="E13" t="s">
+        <v>139</v>
+      </c>
+      <c r="F13">
         <v>11</v>
       </c>
-      <c r="F13" t="s">
-        <v>8</v>
-      </c>
       <c r="G13" t="s">
-        <v>16</v>
+        <v>166</v>
       </c>
       <c r="H13" t="s">
-        <v>18</v>
+        <v>58</v>
       </c>
       <c r="I13" t="s">
-        <v>82</v>
+        <v>10</v>
       </c>
       <c r="J13" t="s">
-        <v>85</v>
-      </c>
-      <c r="K13" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>5</v>
       </c>
@@ -1419,31 +1405,28 @@
         <v>44838</v>
       </c>
       <c r="D14" t="s">
-        <v>62</v>
-      </c>
-      <c r="E14">
+        <v>35</v>
+      </c>
+      <c r="E14" t="s">
+        <v>140</v>
+      </c>
+      <c r="F14">
         <v>12</v>
       </c>
-      <c r="F14" t="s">
-        <v>8</v>
-      </c>
       <c r="G14" t="s">
-        <v>16</v>
+        <v>120</v>
       </c>
       <c r="H14" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="I14" t="s">
-        <v>89</v>
+        <v>10</v>
       </c>
       <c r="J14" t="s">
-        <v>94</v>
-      </c>
-      <c r="K14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>5</v>
       </c>
@@ -1455,31 +1438,28 @@
         <v>44838</v>
       </c>
       <c r="D15" t="s">
-        <v>83</v>
-      </c>
-      <c r="E15">
+        <v>54</v>
+      </c>
+      <c r="E15" t="s">
+        <v>141</v>
+      </c>
+      <c r="F15">
         <v>13</v>
       </c>
-      <c r="F15" t="s">
-        <v>8</v>
-      </c>
       <c r="G15" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="H15" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="I15" t="s">
-        <v>90</v>
+        <v>10</v>
       </c>
       <c r="J15" t="s">
-        <v>95</v>
-      </c>
-      <c r="K15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>5</v>
       </c>
@@ -1491,31 +1471,28 @@
         <v>44840</v>
       </c>
       <c r="D16" t="s">
-        <v>91</v>
-      </c>
-      <c r="E16">
+        <v>59</v>
+      </c>
+      <c r="E16" t="s">
+        <v>142</v>
+      </c>
+      <c r="F16">
         <v>14</v>
       </c>
-      <c r="F16" t="s">
-        <v>8</v>
-      </c>
       <c r="G16" t="s">
-        <v>16</v>
+        <v>166</v>
       </c>
       <c r="H16" t="s">
-        <v>18</v>
+        <v>60</v>
       </c>
       <c r="I16" t="s">
-        <v>92</v>
+        <v>10</v>
       </c>
       <c r="J16" t="s">
-        <v>96</v>
-      </c>
-      <c r="K16" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>6</v>
       </c>
@@ -1527,31 +1504,28 @@
         <v>44845</v>
       </c>
       <c r="D17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17">
+        <v>37</v>
+      </c>
+      <c r="E17" t="s">
+        <v>143</v>
+      </c>
+      <c r="F17">
         <v>15</v>
       </c>
-      <c r="F17" t="s">
-        <v>8</v>
-      </c>
       <c r="G17" t="s">
-        <v>16</v>
+        <v>166</v>
       </c>
       <c r="H17" t="s">
-        <v>18</v>
+        <v>69</v>
       </c>
       <c r="I17" t="s">
-        <v>97</v>
+        <v>10</v>
       </c>
       <c r="J17" t="s">
-        <v>100</v>
-      </c>
-      <c r="K17" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>6</v>
       </c>
@@ -1563,31 +1537,28 @@
         <v>44845</v>
       </c>
       <c r="D18" t="s">
-        <v>65</v>
-      </c>
-      <c r="E18">
+        <v>38</v>
+      </c>
+      <c r="E18" t="s">
+        <v>144</v>
+      </c>
+      <c r="F18">
         <v>16</v>
       </c>
-      <c r="F18" t="s">
-        <v>8</v>
-      </c>
       <c r="G18" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="H18" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
       <c r="I18" t="s">
-        <v>98</v>
+        <v>10</v>
       </c>
       <c r="J18" t="s">
-        <v>101</v>
-      </c>
-      <c r="K18" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>6</v>
       </c>
@@ -1599,31 +1570,28 @@
         <v>44847</v>
       </c>
       <c r="D19" t="s">
-        <v>66</v>
-      </c>
-      <c r="E19">
+        <v>39</v>
+      </c>
+      <c r="E19" t="s">
+        <v>145</v>
+      </c>
+      <c r="F19">
         <v>17</v>
       </c>
-      <c r="F19" t="s">
-        <v>8</v>
-      </c>
       <c r="G19" t="s">
-        <v>16</v>
+        <v>163</v>
       </c>
       <c r="H19" t="s">
-        <v>105</v>
+        <v>71</v>
       </c>
       <c r="I19" t="s">
-        <v>103</v>
+        <v>10</v>
       </c>
       <c r="J19" t="s">
-        <v>102</v>
-      </c>
-      <c r="K19" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>7</v>
       </c>
@@ -1635,31 +1603,28 @@
         <v>44852</v>
       </c>
       <c r="D20" t="s">
-        <v>106</v>
-      </c>
-      <c r="E20">
+        <v>68</v>
+      </c>
+      <c r="E20" t="s">
+        <v>146</v>
+      </c>
+      <c r="F20">
         <v>18</v>
       </c>
-      <c r="F20" t="s">
-        <v>8</v>
-      </c>
       <c r="G20" t="s">
-        <v>16</v>
+        <v>122</v>
       </c>
       <c r="H20" t="s">
-        <v>111</v>
+        <v>72</v>
       </c>
       <c r="I20" t="s">
-        <v>110</v>
+        <v>10</v>
       </c>
       <c r="J20" t="s">
-        <v>113</v>
-      </c>
-      <c r="K20" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>7</v>
       </c>
@@ -1671,31 +1636,28 @@
         <v>44854</v>
       </c>
       <c r="D21" t="s">
-        <v>119</v>
-      </c>
-      <c r="E21">
+        <v>77</v>
+      </c>
+      <c r="E21" t="s">
+        <v>147</v>
+      </c>
+      <c r="F21">
         <v>19</v>
       </c>
-      <c r="F21" t="s">
-        <v>8</v>
-      </c>
       <c r="G21" t="s">
-        <v>16</v>
+        <v>166</v>
       </c>
       <c r="H21" t="s">
-        <v>18</v>
+        <v>75</v>
       </c>
       <c r="I21" t="s">
-        <v>148</v>
+        <v>10</v>
       </c>
       <c r="J21" t="s">
-        <v>159</v>
-      </c>
-      <c r="K21" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>7</v>
       </c>
@@ -1707,31 +1669,28 @@
         <v>44854</v>
       </c>
       <c r="D22" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22">
+        <v>43</v>
+      </c>
+      <c r="E22" t="s">
+        <v>148</v>
+      </c>
+      <c r="F22">
         <v>20</v>
       </c>
-      <c r="F22" t="s">
-        <v>8</v>
-      </c>
       <c r="G22" t="s">
-        <v>16</v>
+        <v>123</v>
       </c>
       <c r="H22" t="s">
-        <v>117</v>
+        <v>76</v>
       </c>
       <c r="I22" t="s">
-        <v>149</v>
+        <v>10</v>
       </c>
       <c r="J22" t="s">
-        <v>160</v>
-      </c>
-      <c r="K22" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>8</v>
       </c>
@@ -1743,46 +1702,49 @@
         <v>44859</v>
       </c>
       <c r="D23" t="s">
-        <v>67</v>
-      </c>
-      <c r="E23">
+        <v>40</v>
+      </c>
+      <c r="E23" t="s">
+        <v>149</v>
+      </c>
+      <c r="F23">
         <v>21</v>
       </c>
-      <c r="F23" t="s">
-        <v>8</v>
-      </c>
       <c r="G23" t="s">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="H23" t="s">
-        <v>134</v>
+        <v>85</v>
       </c>
       <c r="I23" t="s">
-        <v>150</v>
+        <v>10</v>
       </c>
       <c r="J23" t="s">
-        <v>114</v>
-      </c>
-      <c r="K23" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>7</v>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C24" s="1">
         <f t="shared" si="0"/>
-        <v>44852</v>
+        <v>44850</v>
       </c>
       <c r="D24" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+      <c r="G24" t="s">
+        <v>164</v>
+      </c>
+      <c r="H24" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>8</v>
       </c>
@@ -1794,25 +1756,22 @@
         <v>44861</v>
       </c>
       <c r="D25" t="s">
-        <v>68</v>
-      </c>
-      <c r="E25">
+        <v>41</v>
+      </c>
+      <c r="E25" t="s">
+        <v>150</v>
+      </c>
+      <c r="F25">
         <v>22</v>
       </c>
-      <c r="F25" t="s">
-        <v>8</v>
-      </c>
-      <c r="G25" t="s">
-        <v>16</v>
-      </c>
       <c r="I25" t="s">
-        <v>118</v>
+        <v>10</v>
       </c>
       <c r="J25" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>8</v>
       </c>
@@ -1824,31 +1783,28 @@
         <v>44861</v>
       </c>
       <c r="D26" t="s">
-        <v>69</v>
-      </c>
-      <c r="E26">
+        <v>42</v>
+      </c>
+      <c r="E26" t="s">
+        <v>151</v>
+      </c>
+      <c r="F26">
         <v>23</v>
       </c>
-      <c r="F26" t="s">
-        <v>8</v>
-      </c>
       <c r="G26" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="H26" t="s">
-        <v>137</v>
+        <v>86</v>
       </c>
       <c r="I26" t="s">
-        <v>126</v>
+        <v>10</v>
       </c>
       <c r="J26" t="s">
-        <v>154</v>
-      </c>
-      <c r="K26" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>9</v>
       </c>
@@ -1860,31 +1816,28 @@
         <v>44866</v>
       </c>
       <c r="D27" t="s">
-        <v>71</v>
-      </c>
-      <c r="E27">
+        <v>44</v>
+      </c>
+      <c r="E27" t="s">
+        <v>152</v>
+      </c>
+      <c r="F27">
         <v>24</v>
       </c>
-      <c r="F27" t="s">
-        <v>8</v>
-      </c>
       <c r="G27" t="s">
-        <v>16</v>
+        <v>186</v>
       </c>
       <c r="H27" t="s">
-        <v>3</v>
+        <v>185</v>
       </c>
       <c r="I27" t="s">
-        <v>124</v>
+        <v>10</v>
       </c>
       <c r="J27" t="s">
-        <v>155</v>
-      </c>
-      <c r="K27" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>9</v>
       </c>
@@ -1896,25 +1849,22 @@
         <v>44866</v>
       </c>
       <c r="D28" t="s">
-        <v>158</v>
-      </c>
-      <c r="E28">
+        <v>97</v>
+      </c>
+      <c r="E28" t="s">
+        <v>153</v>
+      </c>
+      <c r="F28">
         <v>25</v>
       </c>
-      <c r="F28" t="s">
-        <v>8</v>
-      </c>
-      <c r="G28" t="s">
-        <v>16</v>
-      </c>
       <c r="I28" t="s">
-        <v>157</v>
+        <v>10</v>
       </c>
       <c r="J28" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>9</v>
       </c>
@@ -1926,25 +1876,22 @@
         <v>44868</v>
       </c>
       <c r="D29" t="s">
-        <v>129</v>
-      </c>
-      <c r="E29">
+        <v>82</v>
+      </c>
+      <c r="E29" t="s">
+        <v>154</v>
+      </c>
+      <c r="F29">
         <v>26</v>
       </c>
-      <c r="F29" t="s">
-        <v>8</v>
-      </c>
-      <c r="G29" t="s">
-        <v>16</v>
-      </c>
       <c r="I29" t="s">
-        <v>162</v>
+        <v>10</v>
       </c>
       <c r="J29" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>8</v>
       </c>
@@ -1956,10 +1903,16 @@
         <v>44861</v>
       </c>
       <c r="D30" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+      <c r="G30" t="s">
+        <v>167</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>11</v>
       </c>
@@ -1971,31 +1924,28 @@
         <v>44880</v>
       </c>
       <c r="D31" t="s">
-        <v>72</v>
-      </c>
-      <c r="E31">
+        <v>45</v>
+      </c>
+      <c r="E31" t="s">
+        <v>155</v>
+      </c>
+      <c r="F31">
         <v>27</v>
       </c>
-      <c r="F31" t="s">
-        <v>8</v>
-      </c>
       <c r="G31" t="s">
-        <v>16</v>
+        <v>166</v>
       </c>
       <c r="H31" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
       <c r="I31" t="s">
-        <v>125</v>
+        <v>10</v>
       </c>
       <c r="J31" t="s">
-        <v>166</v>
-      </c>
-      <c r="K31" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>11</v>
       </c>
@@ -2007,31 +1957,28 @@
         <v>44882</v>
       </c>
       <c r="D32" t="s">
-        <v>122</v>
-      </c>
-      <c r="E32">
+        <v>80</v>
+      </c>
+      <c r="E32" t="s">
+        <v>156</v>
+      </c>
+      <c r="F32">
         <v>28</v>
       </c>
-      <c r="F32" t="s">
-        <v>8</v>
-      </c>
       <c r="G32" t="s">
-        <v>16</v>
+        <v>124</v>
       </c>
       <c r="H32" t="s">
-        <v>139</v>
+        <v>88</v>
       </c>
       <c r="I32" t="s">
-        <v>152</v>
+        <v>10</v>
       </c>
       <c r="J32" t="s">
-        <v>165</v>
-      </c>
-      <c r="K32" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>11</v>
       </c>
@@ -2043,31 +1990,28 @@
         <v>44882</v>
       </c>
       <c r="D33" t="s">
-        <v>123</v>
-      </c>
-      <c r="E33">
+        <v>81</v>
+      </c>
+      <c r="E33" t="s">
+        <v>157</v>
+      </c>
+      <c r="F33">
         <v>29</v>
       </c>
-      <c r="F33" t="s">
-        <v>8</v>
-      </c>
       <c r="G33" t="s">
-        <v>16</v>
+        <v>125</v>
       </c>
       <c r="H33" t="s">
-        <v>140</v>
+        <v>89</v>
       </c>
       <c r="I33" t="s">
-        <v>151</v>
+        <v>10</v>
       </c>
       <c r="J33" t="s">
-        <v>164</v>
-      </c>
-      <c r="K33" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>12</v>
       </c>
@@ -2079,31 +2023,28 @@
         <v>44887</v>
       </c>
       <c r="D34" t="s">
-        <v>121</v>
-      </c>
-      <c r="E34">
+        <v>79</v>
+      </c>
+      <c r="E34" t="s">
+        <v>158</v>
+      </c>
+      <c r="F34">
         <v>30</v>
       </c>
-      <c r="F34" t="s">
-        <v>8</v>
-      </c>
       <c r="G34" t="s">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="H34" t="s">
-        <v>143</v>
+        <v>91</v>
       </c>
       <c r="I34" t="s">
-        <v>127</v>
+        <v>10</v>
       </c>
       <c r="J34" t="s">
-        <v>168</v>
-      </c>
-      <c r="K34" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>12</v>
       </c>
@@ -2115,31 +2056,28 @@
         <v>44889</v>
       </c>
       <c r="D35" t="s">
-        <v>120</v>
-      </c>
-      <c r="E35">
+        <v>78</v>
+      </c>
+      <c r="E35" t="s">
+        <v>159</v>
+      </c>
+      <c r="F35">
         <v>31</v>
       </c>
-      <c r="F35" t="s">
-        <v>8</v>
-      </c>
       <c r="G35" t="s">
-        <v>16</v>
+        <v>166</v>
       </c>
       <c r="H35" t="s">
-        <v>18</v>
+        <v>90</v>
       </c>
       <c r="I35" t="s">
-        <v>128</v>
+        <v>10</v>
       </c>
       <c r="J35" t="s">
-        <v>167</v>
-      </c>
-      <c r="K35" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>12</v>
       </c>
@@ -2151,31 +2089,28 @@
         <v>44889</v>
       </c>
       <c r="D36" t="s">
-        <v>73</v>
-      </c>
-      <c r="E36">
+        <v>46</v>
+      </c>
+      <c r="E36" t="s">
+        <v>160</v>
+      </c>
+      <c r="F36">
         <v>32</v>
       </c>
-      <c r="F36" t="s">
-        <v>8</v>
-      </c>
       <c r="G36" t="s">
-        <v>16</v>
+        <v>46</v>
       </c>
       <c r="H36" t="s">
-        <v>144</v>
+        <v>92</v>
       </c>
       <c r="I36" t="s">
-        <v>131</v>
+        <v>10</v>
       </c>
       <c r="J36" t="s">
-        <v>169</v>
-      </c>
-      <c r="K36" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>13</v>
       </c>
@@ -2187,25 +2122,22 @@
         <v>44894</v>
       </c>
       <c r="D37" t="s">
-        <v>74</v>
-      </c>
-      <c r="E37">
+        <v>47</v>
+      </c>
+      <c r="E37" t="s">
+        <v>161</v>
+      </c>
+      <c r="F37">
         <v>33</v>
       </c>
-      <c r="F37" t="s">
-        <v>8</v>
-      </c>
-      <c r="G37" t="s">
-        <v>16</v>
-      </c>
       <c r="I37" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
       <c r="J37" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>13</v>
       </c>
@@ -2217,19 +2149,22 @@
         <v>44894</v>
       </c>
       <c r="D38" t="s">
-        <v>130</v>
-      </c>
-      <c r="E38">
+        <v>83</v>
+      </c>
+      <c r="E38" t="s">
+        <v>162</v>
+      </c>
+      <c r="F38">
         <v>34</v>
       </c>
-      <c r="G38" t="s">
-        <v>16</v>
+      <c r="I38" t="s">
+        <v>10</v>
       </c>
       <c r="J38" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>14</v>
       </c>
@@ -2241,25 +2176,16 @@
         <v>44900</v>
       </c>
       <c r="D39" t="s">
-        <v>40</v>
-      </c>
-      <c r="F39" t="s">
-        <v>10</v>
-      </c>
-      <c r="G39" t="s">
-        <v>174</v>
-      </c>
-      <c r="H39" t="s">
-        <v>173</v>
+        <v>22</v>
+      </c>
+      <c r="I39" t="s">
+        <v>109</v>
       </c>
       <c r="J39" t="s">
-        <v>171</v>
-      </c>
-      <c r="K39" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>14</v>
       </c>
@@ -2271,25 +2197,16 @@
         <v>44901</v>
       </c>
       <c r="D40" t="s">
-        <v>41</v>
-      </c>
-      <c r="F40" t="s">
-        <v>10</v>
-      </c>
-      <c r="G40" t="s">
-        <v>174</v>
-      </c>
-      <c r="H40" t="s">
-        <v>173</v>
+        <v>23</v>
+      </c>
+      <c r="I40" t="s">
+        <v>109</v>
       </c>
       <c r="J40" t="s">
-        <v>171</v>
-      </c>
-      <c r="K40" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>14</v>
       </c>
@@ -2301,10 +2218,16 @@
         <v>44902</v>
       </c>
       <c r="D41" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+      <c r="G41" t="s">
+        <v>169</v>
+      </c>
+      <c r="H41" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>3</v>
       </c>
@@ -2316,10 +2239,16 @@
         <v>44825</v>
       </c>
       <c r="D42" t="s">
+        <v>110</v>
+      </c>
+      <c r="G42" t="s">
+        <v>168</v>
+      </c>
+      <c r="H42" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>5</v>
       </c>
@@ -2331,10 +2260,16 @@
         <v>44839</v>
       </c>
       <c r="D43" t="s">
+        <v>111</v>
+      </c>
+      <c r="G43" t="s">
+        <v>170</v>
+      </c>
+      <c r="H43" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>7</v>
       </c>
@@ -2346,10 +2281,16 @@
         <v>44853</v>
       </c>
       <c r="D44" t="s">
+        <v>112</v>
+      </c>
+      <c r="G44" t="s">
+        <v>171</v>
+      </c>
+      <c r="H44" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>9</v>
       </c>
@@ -2361,10 +2302,16 @@
         <v>44867</v>
       </c>
       <c r="D45" t="s">
+        <v>113</v>
+      </c>
+      <c r="G45" t="s">
+        <v>172</v>
+      </c>
+      <c r="H45" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>12</v>
       </c>
@@ -2376,10 +2323,16 @@
         <v>44888</v>
       </c>
       <c r="D46" t="s">
+        <v>114</v>
+      </c>
+      <c r="G46" t="s">
+        <v>173</v>
+      </c>
+      <c r="H46" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>14</v>
       </c>
@@ -2391,14 +2344,21 @@
         <v>44901</v>
       </c>
       <c r="D47" t="s">
+        <v>115</v>
+      </c>
+      <c r="G47" t="s">
+        <v>174</v>
+      </c>
+      <c r="H47" t="s">
         <v>180</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A17:K41">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A17:J41">
     <sortCondition ref="A17:A41"/>
     <sortCondition ref="B17:B41"/>
   </sortState>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated for weeks 1-3
</commit_message>
<xml_diff>
--- a/data-viz/schedule.xlsx
+++ b/data-viz/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airwin/Dropbox/Teaching/STAT 2430 Data Viz/Data-Viz-2022/Course/data-viz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C010EB28-27A0-5A40-8976-EC72C79880F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F14F88B2-CABF-B942-9B6E-8DF746105049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="30220" windowHeight="19220" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="187">
   <si>
     <t>Date</t>
   </si>
@@ -72,24 +72,12 @@
     <t>slides</t>
   </si>
   <si>
-    <t>slides/00-course-mechanics.html</t>
-  </si>
-  <si>
-    <t>slides/01-invitation.html</t>
-  </si>
-  <si>
     <t>#task-1</t>
   </si>
   <si>
-    <t>slides/02-computer-tools.html</t>
-  </si>
-  <si>
     <t>#task-b1</t>
   </si>
   <si>
-    <t>slides/04-look-at-data.html</t>
-  </si>
-  <si>
     <t>#task-3</t>
   </si>
   <si>
@@ -99,9 +87,6 @@
     <t>Making your first plot</t>
   </si>
   <si>
-    <t>slides/05-making-your-first-plot.html</t>
-  </si>
-  <si>
     <t>Oral presentations, day 1</t>
   </si>
   <si>
@@ -111,9 +96,6 @@
     <t>Version control</t>
   </si>
   <si>
-    <t>slides/06-version-control.html</t>
-  </si>
-  <si>
     <t>Introduction to the grammar of graphics</t>
   </si>
   <si>
@@ -192,24 +174,9 @@
     <t>#task-b4</t>
   </si>
   <si>
-    <t>slides/08-ggplot-intro.html</t>
-  </si>
-  <si>
-    <t>slides/07-grammar-graphics.html</t>
-  </si>
-  <si>
     <t>Displaying tables</t>
   </si>
   <si>
-    <t>slides/10-summarizing-data.html</t>
-  </si>
-  <si>
-    <t>slides/11-reading-data.html</t>
-  </si>
-  <si>
-    <t>slides/09-facets.html</t>
-  </si>
-  <si>
     <t>#task-b5</t>
   </si>
   <si>
@@ -219,27 +186,9 @@
     <t>#task-b6</t>
   </si>
   <si>
-    <t>slides/12-reshaping-data.html</t>
-  </si>
-  <si>
-    <t>slides/13-displaying-tables.html</t>
-  </si>
-  <si>
-    <t>slides/14-getting-help.html</t>
-  </si>
-  <si>
     <t>Project teams sign-up deadline</t>
   </si>
   <si>
-    <t>slides/15-working-with-models.html</t>
-  </si>
-  <si>
-    <t>slides/16-linear-models.html</t>
-  </si>
-  <si>
-    <t>slides/17-gam-loess.html</t>
-  </si>
-  <si>
     <t>Collaboration with GitHub</t>
   </si>
   <si>
@@ -255,12 +204,6 @@
     <t>#task-11</t>
   </si>
   <si>
-    <t>slides/18-collaboration.html</t>
-  </si>
-  <si>
-    <t>slides/19-PCA.html</t>
-  </si>
-  <si>
     <t>#task-b8</t>
   </si>
   <si>
@@ -288,9 +231,6 @@
     <t>Reconstructing a visualization</t>
   </si>
   <si>
-    <t>slides/35-step-by-step.html</t>
-  </si>
-  <si>
     <t>#task-13</t>
   </si>
   <si>
@@ -315,57 +255,12 @@
     <t>#task-18</t>
   </si>
   <si>
-    <t>slides/20-MDS.html</t>
-  </si>
-  <si>
-    <t>slides/21-k-means.html</t>
-  </si>
-  <si>
-    <t>slides/20-slide-presentation.html</t>
-  </si>
-  <si>
-    <t>slides/25-testing.html</t>
-  </si>
-  <si>
     <t>Checking your work</t>
   </si>
   <si>
-    <t>slides/18a-finding-data.html</t>
-  </si>
-  <si>
-    <t>slides/18b-reproducible-reports.html</t>
-  </si>
-  <si>
-    <t>slides/26-dynamic-graphics.html</t>
-  </si>
-  <si>
-    <t>slides/29-map-alternatives.html</t>
-  </si>
-  <si>
-    <t>slides/28-sliding-maps.html</t>
-  </si>
-  <si>
-    <t>slides/27-making-maps.html</t>
-  </si>
-  <si>
-    <t>slides/31-colour.html</t>
-  </si>
-  <si>
-    <t>slides/30-factors-dates.html</t>
-  </si>
-  <si>
-    <t>slides/32-theme.html</t>
-  </si>
-  <si>
-    <t>slides/33-graphics-output.html</t>
-  </si>
-  <si>
     <t>https://github.com/Dalhousie-AndrewIrwin-Teaching/team-planning/blob/main/presentation-schedule.csv</t>
   </si>
   <si>
-    <t>Schedule</t>
-  </si>
-  <si>
     <t>Assignment 1 due</t>
   </si>
   <si>
@@ -595,6 +490,111 @@
   </si>
   <si>
     <t>Presentation</t>
+  </si>
+  <si>
+    <t>01-invitation.html</t>
+  </si>
+  <si>
+    <t>02-computer-tools.html</t>
+  </si>
+  <si>
+    <t>04-look-at-data.html</t>
+  </si>
+  <si>
+    <t>05-making-your-first-plot.html</t>
+  </si>
+  <si>
+    <t>06-version-control.html</t>
+  </si>
+  <si>
+    <t>07-grammar-graphics.html</t>
+  </si>
+  <si>
+    <t>08-ggplot-intro.html</t>
+  </si>
+  <si>
+    <t>10-summarizing-data.html</t>
+  </si>
+  <si>
+    <t>09-facets.html</t>
+  </si>
+  <si>
+    <t>11-reading-data.html</t>
+  </si>
+  <si>
+    <t>12-reshaping-data.html</t>
+  </si>
+  <si>
+    <t>13-displaying-tables.html</t>
+  </si>
+  <si>
+    <t>14-getting-help.html</t>
+  </si>
+  <si>
+    <t>15-working-with-models.html</t>
+  </si>
+  <si>
+    <t>16-linear-models.html</t>
+  </si>
+  <si>
+    <t>17-gam-loess.html</t>
+  </si>
+  <si>
+    <t>18-collaboration.html</t>
+  </si>
+  <si>
+    <t>18a-finding-data.html</t>
+  </si>
+  <si>
+    <t>18b-reproducible-reports.html</t>
+  </si>
+  <si>
+    <t>19-PCA.html</t>
+  </si>
+  <si>
+    <t>20-MDS.html</t>
+  </si>
+  <si>
+    <t>21-k-means.html</t>
+  </si>
+  <si>
+    <t>20-slide-presentation.html</t>
+  </si>
+  <si>
+    <t>25-testing.html</t>
+  </si>
+  <si>
+    <t>26-dynamic-graphics.html</t>
+  </si>
+  <si>
+    <t>27-making-maps.html</t>
+  </si>
+  <si>
+    <t>28-sliding-maps.html</t>
+  </si>
+  <si>
+    <t>29-map-alternatives.html</t>
+  </si>
+  <si>
+    <t>30-factors-dates.html</t>
+  </si>
+  <si>
+    <t>31-colour.html</t>
+  </si>
+  <si>
+    <t>32-theme.html</t>
+  </si>
+  <si>
+    <t>33-graphics-output.html</t>
+  </si>
+  <si>
+    <t>35-step-by-step.html</t>
+  </si>
+  <si>
+    <t>00-course-mechanics.html</t>
+  </si>
+  <si>
+    <t>Live demo</t>
   </si>
 </sst>
 </file>
@@ -967,10 +967,10 @@
   <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E13" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B25" sqref="B25"/>
+      <selection pane="bottomRight" activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -994,19 +994,19 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>127</v>
+        <v>92</v>
       </c>
       <c r="E1" t="s">
-        <v>128</v>
+        <v>93</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>183</v>
+        <v>148</v>
       </c>
       <c r="H1" t="s">
-        <v>184</v>
+        <v>149</v>
       </c>
       <c r="I1" t="s">
         <v>11</v>
@@ -1030,7 +1030,7 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>138</v>
+        <v>103</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -1039,7 +1039,7 @@
         <v>10</v>
       </c>
       <c r="J2" t="s">
-        <v>12</v>
+        <v>185</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -1057,7 +1057,7 @@
         <v>3</v>
       </c>
       <c r="E3" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
       <c r="F3">
         <v>1</v>
@@ -1066,13 +1066,13 @@
         <v>3</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I3" t="s">
         <v>10</v>
       </c>
       <c r="J3" t="s">
-        <v>13</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -1090,22 +1090,22 @@
         <v>5</v>
       </c>
       <c r="E4" t="s">
-        <v>129</v>
+        <v>94</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="I4" t="s">
         <v>10</v>
       </c>
       <c r="J4" t="s">
-        <v>15</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -1123,16 +1123,19 @@
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>130</v>
+        <v>95</v>
       </c>
       <c r="F5">
         <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="H5" t="s">
-        <v>19</v>
+        <v>15</v>
+      </c>
+      <c r="I5" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -1150,22 +1153,22 @@
         <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>131</v>
+        <v>96</v>
       </c>
       <c r="F6">
         <v>4</v>
       </c>
       <c r="G6" t="s">
-        <v>117</v>
+        <v>82</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I6" t="s">
         <v>10</v>
       </c>
       <c r="J6" t="s">
-        <v>17</v>
+        <v>154</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
@@ -1180,25 +1183,25 @@
         <v>44817</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>132</v>
+        <v>97</v>
       </c>
       <c r="F7">
         <v>5</v>
       </c>
       <c r="G7" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="H7" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="I7" t="s">
         <v>10</v>
       </c>
       <c r="J7" t="s">
-        <v>21</v>
+        <v>155</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
@@ -1213,10 +1216,10 @@
         <v>44819</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E8" t="s">
-        <v>133</v>
+        <v>98</v>
       </c>
       <c r="F8">
         <v>6</v>
@@ -1225,7 +1228,7 @@
         <v>10</v>
       </c>
       <c r="J8" t="s">
-        <v>25</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
@@ -1240,25 +1243,25 @@
         <v>44824</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="E9" t="s">
-        <v>134</v>
+        <v>99</v>
       </c>
       <c r="F9">
         <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="H9" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="I9" t="s">
         <v>10</v>
       </c>
       <c r="J9" t="s">
-        <v>53</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
@@ -1273,25 +1276,25 @@
         <v>44824</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>135</v>
+        <v>100</v>
       </c>
       <c r="F10">
         <v>8</v>
       </c>
       <c r="G10" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="H10" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="I10" t="s">
         <v>10</v>
       </c>
       <c r="J10" t="s">
-        <v>52</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -1306,25 +1309,25 @@
         <v>44831</v>
       </c>
       <c r="D11" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="E11" t="s">
-        <v>136</v>
+        <v>101</v>
       </c>
       <c r="F11">
         <v>9</v>
       </c>
       <c r="G11" t="s">
-        <v>118</v>
+        <v>83</v>
       </c>
       <c r="H11" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="I11" t="s">
         <v>10</v>
       </c>
       <c r="J11" t="s">
-        <v>55</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
@@ -1339,25 +1342,25 @@
         <v>44831</v>
       </c>
       <c r="D12" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>137</v>
+        <v>102</v>
       </c>
       <c r="F12">
         <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>119</v>
+        <v>84</v>
       </c>
       <c r="H12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="I12" t="s">
         <v>10</v>
       </c>
       <c r="J12" t="s">
-        <v>57</v>
+        <v>160</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -1372,25 +1375,22 @@
         <v>44833</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E13" t="s">
-        <v>139</v>
+        <v>104</v>
       </c>
       <c r="F13">
         <v>11</v>
       </c>
       <c r="G13" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="H13" t="s">
-        <v>58</v>
-      </c>
-      <c r="I13" t="s">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="J13" t="s">
-        <v>56</v>
+        <v>161</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
@@ -1405,25 +1405,22 @@
         <v>44838</v>
       </c>
       <c r="D14" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E14" t="s">
-        <v>140</v>
+        <v>105</v>
       </c>
       <c r="F14">
         <v>12</v>
       </c>
       <c r="G14" t="s">
-        <v>120</v>
+        <v>85</v>
       </c>
       <c r="H14" t="s">
-        <v>31</v>
-      </c>
-      <c r="I14" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="J14" t="s">
-        <v>61</v>
+        <v>162</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -1438,25 +1435,22 @@
         <v>44838</v>
       </c>
       <c r="D15" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="E15" t="s">
-        <v>141</v>
+        <v>106</v>
       </c>
       <c r="F15">
         <v>13</v>
       </c>
       <c r="G15" t="s">
-        <v>121</v>
+        <v>86</v>
       </c>
       <c r="H15" t="s">
-        <v>32</v>
-      </c>
-      <c r="I15" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="J15" t="s">
-        <v>62</v>
+        <v>163</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -1471,25 +1465,22 @@
         <v>44840</v>
       </c>
       <c r="D16" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="E16" t="s">
-        <v>142</v>
+        <v>107</v>
       </c>
       <c r="F16">
         <v>14</v>
       </c>
       <c r="G16" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="H16" t="s">
-        <v>60</v>
-      </c>
-      <c r="I16" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="J16" t="s">
-        <v>63</v>
+        <v>164</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -1504,25 +1495,22 @@
         <v>44845</v>
       </c>
       <c r="D17" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="E17" t="s">
-        <v>143</v>
+        <v>108</v>
       </c>
       <c r="F17">
         <v>15</v>
       </c>
       <c r="G17" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="H17" t="s">
-        <v>69</v>
-      </c>
-      <c r="I17" t="s">
-        <v>10</v>
+        <v>52</v>
       </c>
       <c r="J17" t="s">
-        <v>65</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -1537,25 +1525,22 @@
         <v>44845</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="E18" t="s">
-        <v>144</v>
+        <v>109</v>
       </c>
       <c r="F18">
         <v>16</v>
       </c>
       <c r="G18" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="H18" t="s">
-        <v>70</v>
-      </c>
-      <c r="I18" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="J18" t="s">
-        <v>66</v>
+        <v>166</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
@@ -1570,25 +1555,22 @@
         <v>44847</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="E19" t="s">
-        <v>145</v>
+        <v>110</v>
       </c>
       <c r="F19">
         <v>17</v>
       </c>
       <c r="G19" t="s">
-        <v>163</v>
+        <v>128</v>
       </c>
       <c r="H19" t="s">
-        <v>71</v>
-      </c>
-      <c r="I19" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="J19" t="s">
-        <v>67</v>
+        <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -1603,25 +1585,22 @@
         <v>44852</v>
       </c>
       <c r="D20" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="E20" t="s">
-        <v>146</v>
+        <v>111</v>
       </c>
       <c r="F20">
         <v>18</v>
       </c>
       <c r="G20" t="s">
-        <v>122</v>
+        <v>87</v>
       </c>
       <c r="H20" t="s">
-        <v>72</v>
-      </c>
-      <c r="I20" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="J20" t="s">
-        <v>73</v>
+        <v>168</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -1636,25 +1615,22 @@
         <v>44854</v>
       </c>
       <c r="D21" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="E21" t="s">
-        <v>147</v>
+        <v>112</v>
       </c>
       <c r="F21">
         <v>19</v>
       </c>
       <c r="G21" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="H21" t="s">
-        <v>75</v>
-      </c>
-      <c r="I21" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="J21" t="s">
-        <v>98</v>
+        <v>169</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -1669,25 +1645,22 @@
         <v>44854</v>
       </c>
       <c r="D22" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="E22" t="s">
-        <v>148</v>
+        <v>113</v>
       </c>
       <c r="F22">
         <v>20</v>
       </c>
       <c r="G22" t="s">
-        <v>123</v>
+        <v>88</v>
       </c>
       <c r="H22" t="s">
-        <v>76</v>
-      </c>
-      <c r="I22" t="s">
-        <v>10</v>
+        <v>57</v>
       </c>
       <c r="J22" t="s">
-        <v>99</v>
+        <v>170</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -1702,25 +1675,22 @@
         <v>44859</v>
       </c>
       <c r="D23" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E23" t="s">
-        <v>149</v>
+        <v>114</v>
       </c>
       <c r="F23">
         <v>21</v>
       </c>
       <c r="G23" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H23" t="s">
-        <v>85</v>
-      </c>
-      <c r="I23" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="J23" t="s">
-        <v>74</v>
+        <v>171</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -1735,13 +1705,13 @@
         <v>44850</v>
       </c>
       <c r="D24" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="G24" t="s">
-        <v>164</v>
+        <v>129</v>
       </c>
       <c r="H24" t="s">
-        <v>165</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
@@ -1756,19 +1726,16 @@
         <v>44861</v>
       </c>
       <c r="D25" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="E25" t="s">
-        <v>150</v>
+        <v>115</v>
       </c>
       <c r="F25">
         <v>22</v>
       </c>
-      <c r="I25" t="s">
-        <v>10</v>
-      </c>
       <c r="J25" t="s">
-        <v>93</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -1783,25 +1750,22 @@
         <v>44861</v>
       </c>
       <c r="D26" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="E26" t="s">
-        <v>151</v>
+        <v>116</v>
       </c>
       <c r="F26">
         <v>23</v>
       </c>
       <c r="G26" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="H26" t="s">
-        <v>86</v>
-      </c>
-      <c r="I26" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="J26" t="s">
-        <v>94</v>
+        <v>173</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
@@ -1816,25 +1780,22 @@
         <v>44866</v>
       </c>
       <c r="D27" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="E27" t="s">
-        <v>152</v>
+        <v>117</v>
       </c>
       <c r="F27">
         <v>24</v>
       </c>
       <c r="G27" t="s">
-        <v>186</v>
+        <v>151</v>
       </c>
       <c r="H27" t="s">
-        <v>185</v>
-      </c>
-      <c r="I27" t="s">
-        <v>10</v>
+        <v>150</v>
       </c>
       <c r="J27" t="s">
-        <v>95</v>
+        <v>174</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -1849,19 +1810,16 @@
         <v>44866</v>
       </c>
       <c r="D28" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="E28" t="s">
-        <v>153</v>
+        <v>118</v>
       </c>
       <c r="F28">
         <v>25</v>
       </c>
-      <c r="I28" t="s">
-        <v>10</v>
-      </c>
       <c r="J28" t="s">
-        <v>96</v>
+        <v>175</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
@@ -1876,19 +1834,16 @@
         <v>44868</v>
       </c>
       <c r="D29" t="s">
-        <v>82</v>
+        <v>63</v>
       </c>
       <c r="E29" t="s">
-        <v>154</v>
+        <v>119</v>
       </c>
       <c r="F29">
         <v>26</v>
       </c>
-      <c r="I29" t="s">
-        <v>10</v>
-      </c>
       <c r="J29" t="s">
-        <v>100</v>
+        <v>176</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
@@ -1903,13 +1858,13 @@
         <v>44861</v>
       </c>
       <c r="D30" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G30" t="s">
-        <v>167</v>
+        <v>132</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>182</v>
+        <v>147</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
@@ -1924,25 +1879,22 @@
         <v>44880</v>
       </c>
       <c r="D31" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E31" t="s">
-        <v>155</v>
+        <v>120</v>
       </c>
       <c r="F31">
         <v>27</v>
       </c>
       <c r="G31" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="H31" t="s">
-        <v>87</v>
-      </c>
-      <c r="I31" t="s">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="J31" t="s">
-        <v>103</v>
+        <v>177</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
@@ -1957,25 +1909,22 @@
         <v>44882</v>
       </c>
       <c r="D32" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="E32" t="s">
-        <v>156</v>
+        <v>121</v>
       </c>
       <c r="F32">
         <v>28</v>
       </c>
       <c r="G32" t="s">
-        <v>124</v>
+        <v>89</v>
       </c>
       <c r="H32" t="s">
-        <v>88</v>
-      </c>
-      <c r="I32" t="s">
-        <v>10</v>
+        <v>68</v>
       </c>
       <c r="J32" t="s">
-        <v>102</v>
+        <v>178</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
@@ -1990,25 +1939,22 @@
         <v>44882</v>
       </c>
       <c r="D33" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="E33" t="s">
-        <v>157</v>
+        <v>122</v>
       </c>
       <c r="F33">
         <v>29</v>
       </c>
       <c r="G33" t="s">
-        <v>125</v>
+        <v>90</v>
       </c>
       <c r="H33" t="s">
-        <v>89</v>
-      </c>
-      <c r="I33" t="s">
-        <v>10</v>
+        <v>69</v>
       </c>
       <c r="J33" t="s">
-        <v>101</v>
+        <v>179</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
@@ -2023,25 +1969,22 @@
         <v>44887</v>
       </c>
       <c r="D34" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="E34" t="s">
-        <v>158</v>
+        <v>123</v>
       </c>
       <c r="F34">
         <v>30</v>
       </c>
       <c r="G34" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="H34" t="s">
-        <v>91</v>
-      </c>
-      <c r="I34" t="s">
-        <v>10</v>
+        <v>71</v>
       </c>
       <c r="J34" t="s">
-        <v>105</v>
+        <v>180</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
@@ -2056,25 +1999,22 @@
         <v>44889</v>
       </c>
       <c r="D35" t="s">
-        <v>78</v>
+        <v>59</v>
       </c>
       <c r="E35" t="s">
-        <v>159</v>
+        <v>124</v>
       </c>
       <c r="F35">
         <v>31</v>
       </c>
       <c r="G35" t="s">
-        <v>166</v>
+        <v>131</v>
       </c>
       <c r="H35" t="s">
-        <v>90</v>
-      </c>
-      <c r="I35" t="s">
-        <v>10</v>
+        <v>70</v>
       </c>
       <c r="J35" t="s">
-        <v>104</v>
+        <v>181</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
@@ -2089,25 +2029,22 @@
         <v>44889</v>
       </c>
       <c r="D36" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E36" t="s">
-        <v>160</v>
+        <v>125</v>
       </c>
       <c r="F36">
         <v>32</v>
       </c>
       <c r="G36" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="H36" t="s">
-        <v>92</v>
-      </c>
-      <c r="I36" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="J36" t="s">
-        <v>106</v>
+        <v>182</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
@@ -2122,19 +2059,16 @@
         <v>44894</v>
       </c>
       <c r="D37" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="E37" t="s">
-        <v>161</v>
+        <v>126</v>
       </c>
       <c r="F37">
         <v>33</v>
       </c>
-      <c r="I37" t="s">
-        <v>10</v>
-      </c>
       <c r="J37" t="s">
-        <v>107</v>
+        <v>183</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
@@ -2149,19 +2083,16 @@
         <v>44894</v>
       </c>
       <c r="D38" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="E38" t="s">
-        <v>162</v>
+        <v>127</v>
       </c>
       <c r="F38">
         <v>34</v>
       </c>
-      <c r="I38" t="s">
-        <v>10</v>
-      </c>
       <c r="J38" t="s">
-        <v>84</v>
+        <v>184</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
@@ -2176,13 +2107,10 @@
         <v>44900</v>
       </c>
       <c r="D39" t="s">
-        <v>22</v>
-      </c>
-      <c r="I39" t="s">
-        <v>109</v>
+        <v>17</v>
       </c>
       <c r="J39" t="s">
-        <v>108</v>
+        <v>74</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
@@ -2197,13 +2125,10 @@
         <v>44901</v>
       </c>
       <c r="D40" t="s">
-        <v>23</v>
-      </c>
-      <c r="I40" t="s">
-        <v>109</v>
+        <v>18</v>
       </c>
       <c r="J40" t="s">
-        <v>108</v>
+        <v>74</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
@@ -2218,13 +2143,13 @@
         <v>44902</v>
       </c>
       <c r="D41" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="G41" t="s">
-        <v>169</v>
+        <v>134</v>
       </c>
       <c r="H41" t="s">
-        <v>181</v>
+        <v>146</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
@@ -2239,13 +2164,13 @@
         <v>44825</v>
       </c>
       <c r="D42" t="s">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="G42" t="s">
-        <v>168</v>
+        <v>133</v>
       </c>
       <c r="H42" t="s">
-        <v>175</v>
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
@@ -2260,13 +2185,13 @@
         <v>44839</v>
       </c>
       <c r="D43" t="s">
-        <v>111</v>
+        <v>76</v>
       </c>
       <c r="G43" t="s">
-        <v>170</v>
+        <v>135</v>
       </c>
       <c r="H43" t="s">
-        <v>176</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
@@ -2281,13 +2206,13 @@
         <v>44853</v>
       </c>
       <c r="D44" t="s">
-        <v>112</v>
+        <v>77</v>
       </c>
       <c r="G44" t="s">
-        <v>171</v>
+        <v>136</v>
       </c>
       <c r="H44" t="s">
-        <v>177</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
@@ -2302,13 +2227,13 @@
         <v>44867</v>
       </c>
       <c r="D45" t="s">
-        <v>113</v>
+        <v>78</v>
       </c>
       <c r="G45" t="s">
-        <v>172</v>
+        <v>137</v>
       </c>
       <c r="H45" t="s">
-        <v>178</v>
+        <v>143</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
@@ -2323,13 +2248,13 @@
         <v>44888</v>
       </c>
       <c r="D46" t="s">
-        <v>114</v>
+        <v>79</v>
       </c>
       <c r="G46" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
       <c r="H46" t="s">
-        <v>179</v>
+        <v>144</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
@@ -2344,13 +2269,13 @@
         <v>44901</v>
       </c>
       <c r="D47" t="s">
-        <v>115</v>
+        <v>80</v>
       </c>
       <c r="G47" t="s">
-        <v>174</v>
+        <v>139</v>
       </c>
       <c r="H47" t="s">
-        <v>180</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test live coding page
</commit_message>
<xml_diff>
--- a/data-viz/schedule.xlsx
+++ b/data-viz/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airwin/Dropbox/Teaching/STAT 2430 Data Viz/Data-Viz-2022/Course/data-viz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7916DC0B-C544-804C-B240-FDCAD1BCA69D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42539936-70A7-3E43-9723-BEBD8C2EC43B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="192">
   <si>
     <t>Date</t>
   </si>
@@ -598,6 +598,18 @@
   </si>
   <si>
     <t>#oral-presentation</t>
+  </si>
+  <si>
+    <t>demo</t>
+  </si>
+  <si>
+    <t>demo_link</t>
+  </si>
+  <si>
+    <t>Demo</t>
+  </si>
+  <si>
+    <t>01-intro-tools</t>
   </si>
 </sst>
 </file>
@@ -967,13 +979,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5054E2AF-B146-EF4C-9336-1C427A68EF7D}">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:L47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E24" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G40" sqref="G40"/>
+      <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -986,7 +998,7 @@
     <col min="10" max="10" width="19.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1017,8 +1029,14 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" t="s">
+        <v>188</v>
+      </c>
+      <c r="L1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1045,7 +1063,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1078,7 +1096,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1111,7 +1129,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1140,8 +1158,14 @@
       <c r="I5" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5" t="s">
+        <v>190</v>
+      </c>
+      <c r="L5" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1174,7 +1198,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1207,7 +1231,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1234,7 +1258,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1267,7 +1291,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1300,7 +1324,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>4</v>
       </c>
@@ -1333,7 +1357,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>4</v>
       </c>
@@ -1366,7 +1390,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1396,7 +1420,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>5</v>
       </c>
@@ -1426,7 +1450,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>5</v>
       </c>
@@ -1456,7 +1480,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Fixing links to Demo slides
</commit_message>
<xml_diff>
--- a/data-viz/schedule.xlsx
+++ b/data-viz/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airwin/Dropbox/Teaching/STAT 2430 Data Viz/Data-Viz-2022/Course/data-viz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42539936-70A7-3E43-9723-BEBD8C2EC43B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BBE2F2C-8F58-8546-BADC-50215C9CF7DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16180" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="194">
   <si>
     <t>Date</t>
   </si>
@@ -609,7 +609,13 @@
     <t>Demo</t>
   </si>
   <si>
-    <t>01-intro-tools</t>
+    <t>03-intro-tools</t>
+  </si>
+  <si>
+    <t>05-first-plot</t>
+  </si>
+  <si>
+    <t>06-version-control</t>
   </si>
 </sst>
 </file>
@@ -985,7 +991,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
+      <selection pane="bottomRight" activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1230,6 +1236,12 @@
       <c r="J7" t="s">
         <v>152</v>
       </c>
+      <c r="K7" t="s">
+        <v>190</v>
+      </c>
+      <c r="L7" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
@@ -1256,6 +1268,12 @@
       </c>
       <c r="J8" t="s">
         <v>153</v>
+      </c>
+      <c r="K8" t="s">
+        <v>190</v>
+      </c>
+      <c r="L8" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Adding a coupe of lectures
</commit_message>
<xml_diff>
--- a/data-viz/schedule.xlsx
+++ b/data-viz/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airwin/Dropbox/Teaching/STAT 2430 Data Viz/Data-Viz-2022/Course/data-viz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865341B5-4D82-E244-A6DF-53B10D3507BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D11B6C-6571-1449-9A4C-CA7F9433D3EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
+    <workbookView xWindow="-35840" yWindow="260" windowWidth="28800" windowHeight="16280" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="202">
   <si>
     <t>Date</t>
   </si>
@@ -1029,7 +1029,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E11" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
+      <selection pane="bottomRight" activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1595,7 +1595,9 @@
       <c r="H17" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I17" s="2"/>
+      <c r="I17" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="J17" s="2" t="s">
         <v>158</v>
       </c>
@@ -1651,7 +1653,9 @@
       <c r="H19" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I19" s="2"/>
+      <c r="I19" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="J19" s="2" t="s">
         <v>159</v>
       </c>

</xml_diff>

<commit_message>
slides up to lesson 20
</commit_message>
<xml_diff>
--- a/data-viz/schedule.xlsx
+++ b/data-viz/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airwin/Dropbox/Teaching/STAT 2430 Data Viz/Data-Viz-2022/Course/data-viz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3D11B6C-6571-1449-9A4C-CA7F9433D3EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A73D630D-DAA2-834D-AE8F-3027BD1F6B88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-35840" yWindow="260" windowWidth="28800" windowHeight="16280" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
+    <workbookView xWindow="4800" yWindow="1800" windowWidth="28800" windowHeight="18000" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="202">
   <si>
     <t>Date</t>
   </si>
@@ -534,12 +534,6 @@
     <t>18-collaboration.html</t>
   </si>
   <si>
-    <t>18a-finding-data.html</t>
-  </si>
-  <si>
-    <t>18b-reproducible-reports.html</t>
-  </si>
-  <si>
     <t>19-PCA.html</t>
   </si>
   <si>
@@ -640,6 +634,12 @@
   </si>
   <si>
     <t>09-summarize</t>
+  </si>
+  <si>
+    <t>19-finding-data.html</t>
+  </si>
+  <si>
+    <t>20-reproducible-reports.html</t>
   </si>
 </sst>
 </file>
@@ -1026,10 +1026,10 @@
   <dimension ref="A1:L53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E11" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E26" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I20" sqref="I20"/>
+      <selection pane="bottomRight" activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1074,10 +1074,10 @@
         <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -1106,7 +1106,7 @@
         <v>10</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -1208,14 +1208,14 @@
         <v>15</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -1286,10 +1286,10 @@
         <v>152</v>
       </c>
       <c r="K7" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="L7" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -1321,10 +1321,10 @@
         <v>153</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -1339,7 +1339,7 @@
         <v>44823</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -1459,7 +1459,7 @@
         <v>44826</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -1468,10 +1468,10 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -1486,7 +1486,7 @@
         <v>44831</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -1530,10 +1530,10 @@
         <v>156</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -1616,7 +1616,7 @@
         <v>44834</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -1664,14 +1664,14 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B20" s="2">
         <v>3</v>
       </c>
       <c r="C20" s="3">
         <f t="shared" si="0"/>
-        <v>44839</v>
+        <v>44846</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>73</v>
@@ -1715,7 +1715,9 @@
       <c r="H21" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I21" s="2"/>
+      <c r="I21" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="J21" s="2" t="s">
         <v>160</v>
       </c>
@@ -1748,7 +1750,9 @@
       <c r="H22" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I22" s="2"/>
+      <c r="I22" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="J22" s="2" t="s">
         <v>161</v>
       </c>
@@ -1767,7 +1771,7 @@
         <v>44844</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -1804,7 +1808,9 @@
       <c r="H24" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="I24" s="2"/>
+      <c r="I24" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="J24" s="2" t="s">
         <v>162</v>
       </c>
@@ -1837,7 +1843,9 @@
       <c r="H25" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I25" s="2"/>
+      <c r="I25" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="J25" s="2" t="s">
         <v>163</v>
       </c>
@@ -1870,7 +1878,9 @@
       <c r="H26" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I26" s="2"/>
+      <c r="I26" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="J26" s="2" t="s">
         <v>164</v>
       </c>
@@ -1930,7 +1940,9 @@
       <c r="H28" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="I28" s="2"/>
+      <c r="I28" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="J28" s="2" t="s">
         <v>165</v>
       </c>
@@ -1990,9 +2002,11 @@
       <c r="H30" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I30" s="2"/>
+      <c r="I30" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="J30" s="2" t="s">
-        <v>166</v>
+        <v>200</v>
       </c>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
@@ -2023,9 +2037,11 @@
       <c r="H31" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="I31" s="2"/>
+      <c r="I31" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="J31" s="2" t="s">
-        <v>167</v>
+        <v>201</v>
       </c>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
@@ -2058,7 +2074,7 @@
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
@@ -2087,7 +2103,7 @@
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
@@ -2120,7 +2136,7 @@
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
@@ -2180,7 +2196,7 @@
       </c>
       <c r="I36" s="2"/>
       <c r="J36" s="2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
@@ -2236,7 +2252,7 @@
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
@@ -2265,7 +2281,7 @@
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
@@ -2282,7 +2298,7 @@
         <v>44876</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
@@ -2321,7 +2337,7 @@
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
@@ -2354,7 +2370,7 @@
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
@@ -2387,7 +2403,7 @@
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
@@ -2420,7 +2436,7 @@
       </c>
       <c r="I44" s="2"/>
       <c r="J44" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
@@ -2480,7 +2496,7 @@
       </c>
       <c r="I46" s="2"/>
       <c r="J46" s="2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
@@ -2513,7 +2529,7 @@
       </c>
       <c r="I47" s="2"/>
       <c r="J47" s="2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
@@ -2542,7 +2558,7 @@
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
@@ -2571,7 +2587,7 @@
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
       <c r="J49" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
@@ -2588,15 +2604,15 @@
         <v>44894</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
@@ -2615,7 +2631,7 @@
         <v>44896</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>

</xml_diff>

<commit_message>
Reports live coding, other fixes
</commit_message>
<xml_diff>
--- a/data-viz/schedule.xlsx
+++ b/data-viz/schedule.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airwin/Dropbox/Teaching/STAT 2430 Data Viz/Data-Viz-2022/Course/data-viz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951640D9-261F-AD4A-93CF-705DE9FD91C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C666C11-953C-564E-A661-40D867FC2A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-35300" yWindow="-780" windowWidth="28800" windowHeight="18000" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="204">
   <si>
     <t>Date</t>
   </si>
@@ -288,9 +288,6 @@
     <t>Tables</t>
   </si>
   <si>
-    <t>Collaboration</t>
-  </si>
-  <si>
     <t>Reports</t>
   </si>
   <si>
@@ -643,6 +640,12 @@
   </si>
   <si>
     <t>15-working-models</t>
+  </si>
+  <si>
+    <t>&lt;i&gt;Bonus task&lt;/i&gt;: Collaboration</t>
+  </si>
+  <si>
+    <t>20-reports</t>
   </si>
 </sst>
 </file>
@@ -1029,10 +1032,10 @@
   <dimension ref="A1:L53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E10" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E17" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K25" sqref="K25"/>
+      <selection pane="bottomRight" activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1056,19 +1059,19 @@
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>146</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>11</v>
@@ -1077,10 +1080,10 @@
         <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>186</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
@@ -1098,7 +1101,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F2" s="2">
         <v>0</v>
@@ -1109,7 +1112,7 @@
         <v>10</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -1129,7 +1132,7 @@
         <v>3</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F3" s="2">
         <v>1</v>
@@ -1144,7 +1147,7 @@
         <v>10</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
@@ -1164,13 +1167,13 @@
         <v>5</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F4" s="2">
         <v>2</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>13</v>
@@ -1179,7 +1182,7 @@
         <v>10</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
@@ -1199,7 +1202,7 @@
         <v>7</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F5" s="2">
         <v>3</v>
@@ -1211,14 +1214,14 @@
         <v>15</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="L5" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -1236,7 +1239,7 @@
         <v>8</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F6" s="2">
         <v>4</v>
@@ -1251,7 +1254,7 @@
         <v>10</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -1271,13 +1274,13 @@
         <v>16</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F7" s="2">
         <v>5</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>20</v>
@@ -1286,13 +1289,13 @@
         <v>10</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -1310,7 +1313,7 @@
         <v>17</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F8" s="2">
         <v>6</v>
@@ -1321,13 +1324,13 @@
         <v>10</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -1342,7 +1345,7 @@
         <v>44823</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -1368,13 +1371,13 @@
         <v>18</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F10" s="2">
         <v>7</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>42</v>
@@ -1383,7 +1386,7 @@
         <v>10</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -1403,13 +1406,13 @@
         <v>19</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F11" s="2">
         <v>8</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>43</v>
@@ -1418,7 +1421,7 @@
         <v>10</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
@@ -1440,10 +1443,10 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -1462,7 +1465,7 @@
         <v>44826</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -1471,10 +1474,10 @@
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -1489,7 +1492,7 @@
         <v>44831</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -1515,7 +1518,7 @@
         <v>25</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F15" s="2">
         <v>9</v>
@@ -1530,13 +1533,13 @@
         <v>10</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -1554,7 +1557,7 @@
         <v>28</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F16" s="2">
         <v>10</v>
@@ -1569,7 +1572,7 @@
         <v>10</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -1587,13 +1590,13 @@
         <v>26</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F17" s="2">
         <v>11</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H17" s="2" t="s">
         <v>45</v>
@@ -1602,7 +1605,7 @@
         <v>10</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
@@ -1619,7 +1622,7 @@
         <v>44834</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -1645,7 +1648,7 @@
         <v>27</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F19" s="2">
         <v>12</v>
@@ -1660,7 +1663,7 @@
         <v>10</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
@@ -1682,10 +1685,10 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -1707,7 +1710,7 @@
         <v>44</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F21" s="2">
         <v>13</v>
@@ -1722,7 +1725,7 @@
         <v>10</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
@@ -1742,13 +1745,13 @@
         <v>46</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F22" s="2">
         <v>14</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H22" s="2" t="s">
         <v>47</v>
@@ -1757,7 +1760,7 @@
         <v>10</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
@@ -1774,7 +1777,7 @@
         <v>44844</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
@@ -1800,13 +1803,13 @@
         <v>29</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F24" s="2">
         <v>15</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>50</v>
@@ -1815,13 +1818,13 @@
         <v>10</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
@@ -1839,7 +1842,7 @@
         <v>30</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F25" s="2">
         <v>16</v>
@@ -1854,7 +1857,7 @@
         <v>10</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
@@ -1874,13 +1877,13 @@
         <v>31</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F26" s="2">
         <v>17</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>52</v>
@@ -1889,7 +1892,7 @@
         <v>10</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
@@ -1911,10 +1914,10 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>126</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>127</v>
       </c>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
@@ -1936,13 +1939,13 @@
         <v>49</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F28" s="2">
         <v>18</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>84</v>
+        <v>202</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>53</v>
@@ -1951,7 +1954,7 @@
         <v>10</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
@@ -1973,10 +1976,10 @@
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -1998,13 +2001,13 @@
         <v>56</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F30" s="2">
         <v>19</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>54</v>
@@ -2013,7 +2016,7 @@
         <v>10</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
@@ -2033,13 +2036,13 @@
         <v>35</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F31" s="2">
         <v>20</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>55</v>
@@ -2048,10 +2051,14 @@
         <v>10</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="K31" s="2"/>
-      <c r="L31" s="2"/>
+        <v>200</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
@@ -2068,7 +2075,7 @@
         <v>32</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F32" s="2">
         <v>21</v>
@@ -2081,7 +2088,7 @@
       </c>
       <c r="I32" s="2"/>
       <c r="J32" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
@@ -2101,7 +2108,7 @@
         <v>33</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F33" s="2">
         <v>22</v>
@@ -2110,7 +2117,7 @@
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
@@ -2130,7 +2137,7 @@
         <v>34</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F34" s="2">
         <v>23</v>
@@ -2143,7 +2150,7 @@
       </c>
       <c r="I34" s="2"/>
       <c r="J34" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
@@ -2165,10 +2172,10 @@
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
@@ -2190,20 +2197,20 @@
         <v>36</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F36" s="2">
         <v>24</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I36" s="2"/>
       <c r="J36" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
@@ -2225,10 +2232,10 @@
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
@@ -2250,7 +2257,7 @@
         <v>71</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F38" s="2">
         <v>25</v>
@@ -2259,7 +2266,7 @@
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="K38" s="2"/>
       <c r="L38" s="2"/>
@@ -2279,7 +2286,7 @@
         <v>61</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F39" s="2">
         <v>26</v>
@@ -2288,7 +2295,7 @@
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
       <c r="J39" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K39" s="2"/>
       <c r="L39" s="2"/>
@@ -2305,7 +2312,7 @@
         <v>44876</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
@@ -2331,20 +2338,20 @@
         <v>37</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F41" s="2">
         <v>27</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>65</v>
       </c>
       <c r="I41" s="2"/>
       <c r="J41" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="K41" s="2"/>
       <c r="L41" s="2"/>
@@ -2364,20 +2371,20 @@
         <v>59</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F42" s="2">
         <v>28</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>66</v>
       </c>
       <c r="I42" s="2"/>
       <c r="J42" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="K42" s="2"/>
       <c r="L42" s="2"/>
@@ -2397,20 +2404,20 @@
         <v>60</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F43" s="2">
         <v>29</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H43" s="2" t="s">
         <v>67</v>
       </c>
       <c r="I43" s="2"/>
       <c r="J43" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="K43" s="2"/>
       <c r="L43" s="2"/>
@@ -2430,7 +2437,7 @@
         <v>58</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F44" s="2">
         <v>30</v>
@@ -2443,7 +2450,7 @@
       </c>
       <c r="I44" s="2"/>
       <c r="J44" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="K44" s="2"/>
       <c r="L44" s="2"/>
@@ -2465,10 +2472,10 @@
       <c r="E45" s="2"/>
       <c r="F45" s="2"/>
       <c r="G45" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I45" s="2"/>
       <c r="J45" s="2"/>
@@ -2490,20 +2497,20 @@
         <v>57</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F46" s="2">
         <v>31</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="H46" s="2" t="s">
         <v>68</v>
       </c>
       <c r="I46" s="2"/>
       <c r="J46" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="K46" s="2"/>
       <c r="L46" s="2"/>
@@ -2523,7 +2530,7 @@
         <v>38</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F47" s="2">
         <v>32</v>
@@ -2536,7 +2543,7 @@
       </c>
       <c r="I47" s="2"/>
       <c r="J47" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="K47" s="2"/>
       <c r="L47" s="2"/>
@@ -2556,7 +2563,7 @@
         <v>39</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F48" s="2">
         <v>33</v>
@@ -2565,7 +2572,7 @@
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
       <c r="J48" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
@@ -2585,7 +2592,7 @@
         <v>62</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F49" s="2">
         <v>34</v>
@@ -2594,7 +2601,7 @@
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
       <c r="J49" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K49" s="2"/>
       <c r="L49" s="2"/>
@@ -2611,15 +2618,15 @@
         <v>44894</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" s="2"/>
       <c r="G50" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="H50" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="H50" s="2" t="s">
-        <v>185</v>
       </c>
       <c r="I50" s="2"/>
       <c r="J50" s="2"/>
@@ -2638,7 +2645,7 @@
         <v>44896</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2"/>
@@ -2666,10 +2673,10 @@
       <c r="E52" s="2"/>
       <c r="F52" s="2"/>
       <c r="G52" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="I52" s="2"/>
       <c r="J52" s="2"/>
@@ -2693,10 +2700,10 @@
       <c r="E53" s="2"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>

</xml_diff>

<commit_message>
live coding update  +slides
</commit_message>
<xml_diff>
--- a/data-viz/schedule.xlsx
+++ b/data-viz/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airwin/Dropbox/Teaching/STAT 2430 Data Viz/Data-Viz-2022/Course/data-viz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{145EB3FB-F3DE-8B4E-A484-41D7DABDFE69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD19EC60-8873-8A41-9354-A698F39EEE28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26520" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="205">
   <si>
     <t>Date</t>
   </si>
@@ -646,6 +646,9 @@
   </si>
   <si>
     <t>34-step-by-step.html</t>
+  </si>
+  <si>
+    <t>21-PCA</t>
   </si>
 </sst>
 </file>
@@ -1035,7 +1038,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="E17" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I35" sqref="I35"/>
+      <selection pane="bottomRight" activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2080,20 +2083,20 @@
       <c r="F32" s="2">
         <v>21</v>
       </c>
-      <c r="G32" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>63</v>
-      </c>
+      <c r="G32" s="2"/>
+      <c r="H32" s="2"/>
       <c r="I32" s="2" t="s">
         <v>10</v>
       </c>
       <c r="J32" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
+      <c r="K32" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>204</v>
+      </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
@@ -2115,8 +2118,12 @@
       <c r="F33" s="2">
         <v>22</v>
       </c>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
+      <c r="G33" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="I33" s="2" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
last week of slides
</commit_message>
<xml_diff>
--- a/data-viz/schedule.xlsx
+++ b/data-viz/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airwin/Dropbox/Teaching/STAT 2430 Data Viz/Data-Viz-2022/Course/data-viz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0B4393-EF26-984B-A28A-E2F145294D0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6433C04-3457-954F-91E9-54A3493D3B0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26520" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
+    <workbookView xWindow="-30720" yWindow="-2040" windowWidth="28800" windowHeight="18000" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="212">
   <si>
     <t>Date</t>
   </si>
@@ -655,6 +655,21 @@
   </si>
   <si>
     <t>27-maps-1</t>
+  </si>
+  <si>
+    <t>28-maps-2</t>
+  </si>
+  <si>
+    <t>31-colour</t>
+  </si>
+  <si>
+    <t>30-factors-dates</t>
+  </si>
+  <si>
+    <t>32-theme</t>
+  </si>
+  <si>
+    <t>33-graphics</t>
   </si>
 </sst>
 </file>
@@ -1041,10 +1056,10 @@
   <dimension ref="A1:L53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E17" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E26" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K42" sqref="K42"/>
+      <selection pane="bottomRight" activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2423,8 +2438,12 @@
       <c r="J42" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
+      <c r="K42" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="L42" s="2" t="s">
+        <v>207</v>
+      </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
@@ -2493,8 +2512,12 @@
       <c r="J44" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="K44" s="2"/>
-      <c r="L44" s="2"/>
+      <c r="K44" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
@@ -2555,8 +2578,12 @@
       <c r="J46" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
+      <c r="K46" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="L46" s="2" t="s">
+        <v>208</v>
+      </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
@@ -2590,8 +2617,12 @@
       <c r="J47" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="K47" s="2"/>
-      <c r="L47" s="2"/>
+      <c r="K47" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
@@ -2621,8 +2652,12 @@
       <c r="J48" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="K48" s="2"/>
-      <c r="L48" s="2"/>
+      <c r="K48" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="L48" s="2" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="2">

</xml_diff>

<commit_message>
fix problem with schedule
</commit_message>
<xml_diff>
--- a/data-viz/schedule.xlsx
+++ b/data-viz/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/airwin/Library/CloudStorage/Dropbox/Teaching/STAT 2430 Data Viz/2024W/data-viz-course/data-viz/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65B673C-C2E9-334F-9A46-02970A342961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DBCBD0E-5E57-DA49-B31E-E310EF370DB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19540" xr2:uid="{D262D957-99A2-4240-BB5D-74EA57927089}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="207">
   <si>
     <t>Date</t>
   </si>
@@ -631,9 +631,6 @@
   </si>
   <si>
     <t>Reading week, no classses</t>
-  </si>
-  <si>
-    <t>Exam period</t>
   </si>
   <si>
     <t>Using R</t>
@@ -1037,10 +1034,10 @@
   <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="E12" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E42" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B26" sqref="B26"/>
+      <selection pane="bottomRight" activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1176,7 +1173,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H4" s="2" t="s">
         <v>13</v>
@@ -1283,7 +1280,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H7" s="2" t="s">
         <v>20</v>
@@ -1322,7 +1319,7 @@
         <v>6</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2" t="s">
@@ -1359,7 +1356,7 @@
         <v>7</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>42</v>
@@ -1394,7 +1391,7 @@
         <v>8</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>43</v>
@@ -1513,7 +1510,7 @@
         <v>45323</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -2606,7 +2603,7 @@
         <v>45386</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2"/>
@@ -2640,12 +2637,9 @@
       <c r="K48" s="2"/>
       <c r="L48" s="2"/>
     </row>
-    <row r="49" spans="3:8" x14ac:dyDescent="0.2">
-      <c r="C49" s="1" t="s">
-        <v>199</v>
-      </c>
+    <row r="49" spans="4:8" x14ac:dyDescent="0.2">
       <c r="D49" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>127</v>

</xml_diff>